<commit_message>
change result file，highlight size
</commit_message>
<xml_diff>
--- a/BulkCreativeImportTemplate.v28.xlsx
+++ b/BulkCreativeImportTemplate.v28.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\adplatform-iii\UI\TradeDeskWeb\TradeDeskWeb\Content\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boya.zeng\PycharmProjects\Creative Creation Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C5DD08-F33D-438B-9765-9AA1E0802199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD96E75-7413-4E2D-BED8-80478C19D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15540" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hosted Display" sheetId="6" r:id="rId1"/>
@@ -122,7 +122,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -137,7 +137,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -152,7 +152,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -168,7 +168,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -274,7 +274,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -290,7 +290,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -316,7 +316,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>[Optional] Indicate whether this creative can be served securely via HTTPS.  Use yes/no to indicate if the creative is securable (blank is interpreted as "yes").</t>
         </r>
@@ -328,7 +328,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -344,7 +344,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -514,7 +514,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -528,7 +528,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -542,7 +542,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -556,7 +556,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -570,7 +570,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -584,7 +584,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -598,7 +598,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -662,7 +662,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -677,7 +677,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -692,7 +692,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -708,7 +708,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -747,7 +747,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -761,7 +761,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -775,7 +775,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -789,7 +789,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -803,7 +803,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -817,7 +817,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -831,7 +831,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -845,7 +845,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -859,7 +859,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -914,7 +914,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -929,7 +929,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -944,7 +944,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -960,7 +960,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -999,7 +999,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1013,7 +1013,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1027,7 +1027,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1041,7 +1041,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1055,7 +1055,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1069,7 +1069,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1083,7 +1083,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1097,7 +1097,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1152,7 +1152,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1168,7 +1168,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -1352,7 +1352,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1368,7 +1368,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -1407,15 +1407,28 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Enabling this tracking feature will provide MOAT video viewability and player size reporting within The Trade Desk's omnichannel dashboards and reports, for this 3rd party video creative.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Enabling this tracking feature will provide MOAT video viewability and player size reporting within The Trade Desk's omnichannel dashboards and reports, for this 3rd party video creative.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
+          </rPr>
+          <t xml:space="preserve"> [Optional] The date the creative will be available to start serving.  If a time is not given, serving will start at 12:00AM on that day in the time zone provided.  If no date is given, the creative will be available to server immediately upon approval.  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1424,11 +1437,11 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> [Optional] The date the creative will be available to start serving.  If a time is not given, serving will start at 12:00AM on that day in the time zone provided.  If no date is given, the creative will be available to server immediately upon approval.  </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
+          <t xml:space="preserve">[Optional] The date after which the creative will no longer be available to serve.  If time is not given, serving will stop at 11:59PM on this day in the time zone provided.  If no date is given, the creative will be indefinitely by default. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1437,19 +1450,6 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[Optional] The date after which the creative will no longer be available to serve.  If time is not given, serving will stop at 11:59PM on this day in the time zone provided.  If no date is given, the creative will be indefinitely by default. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">[Required if flight dates exist]  Use the “Time Zone Declarations” tab in this document to determine the time zone ID. Enter the text ID describing the time zone for the flight dates. </t>
         </r>
       </text>
@@ -1460,7 +1460,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1476,7 +1476,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -1516,7 +1516,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1530,7 +1530,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1544,7 +1544,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1558,7 +1558,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1572,7 +1572,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1586,7 +1586,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1600,7 +1600,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1655,7 +1655,7 @@
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <rFont val="宋体"/>
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
@@ -1671,7 +1671,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Comma separated list
 </t>
@@ -2794,13 +2794,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2808,7 +2808,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2816,7 +2816,7 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2824,7 +2824,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2832,7 +2832,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2852,14 +2852,14 @@
     <font>
       <sz val="9"/>
       <color indexed="81"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2878,9 +2878,10 @@
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2972,8 +2973,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -3259,13 +3260,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="26.453125" customWidth="1"/>
@@ -3278,7 +3279,7 @@
     <col min="21" max="21" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>320</v>
       </c>
@@ -3344,6 +3345,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -3368,13 +3370,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>310</v>
       </c>
@@ -3382,7 +3384,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>243</v>
       </c>
@@ -3390,7 +3392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -3398,7 +3400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>241</v>
       </c>
@@ -3406,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>270</v>
       </c>
@@ -3414,7 +3416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -3422,7 +3424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>288</v>
       </c>
@@ -3430,7 +3432,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>244</v>
       </c>
@@ -3446,7 +3448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>246</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>293</v>
       </c>
@@ -3462,7 +3464,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>264</v>
       </c>
@@ -3470,7 +3472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -3478,7 +3480,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>284</v>
       </c>
@@ -3486,7 +3488,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>247</v>
       </c>
@@ -3494,7 +3496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -3502,7 +3504,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>272</v>
       </c>
@@ -3510,7 +3512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>248</v>
       </c>
@@ -3518,7 +3520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>296</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>249</v>
       </c>
@@ -3534,7 +3536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>290</v>
       </c>
@@ -3542,7 +3544,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>250</v>
       </c>
@@ -3550,7 +3552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>258</v>
       </c>
@@ -3558,7 +3560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -3566,7 +3568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>291</v>
       </c>
@@ -3574,7 +3576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>282</v>
       </c>
@@ -3582,7 +3584,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -3590,7 +3592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>275</v>
       </c>
@@ -3598,7 +3600,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>285</v>
       </c>
@@ -3606,7 +3608,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>268</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>252</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>253</v>
       </c>
@@ -3630,7 +3632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>254</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>287</v>
       </c>
@@ -3646,7 +3648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>269</v>
       </c>
@@ -3654,7 +3656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>255</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>256</v>
       </c>
@@ -3670,7 +3672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>267</v>
       </c>
@@ -3678,7 +3680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>292</v>
       </c>
@@ -3686,7 +3688,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>283</v>
       </c>
@@ -3694,7 +3696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>257</v>
       </c>
@@ -3702,7 +3704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>295</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>294</v>
       </c>
@@ -3718,7 +3720,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>297</v>
       </c>
@@ -3726,7 +3728,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>278</v>
       </c>
@@ -3734,7 +3736,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>280</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>259</v>
       </c>
@@ -3750,7 +3752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>260</v>
       </c>
@@ -3758,7 +3760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>286</v>
       </c>
@@ -3766,7 +3768,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>276</v>
       </c>
@@ -3774,7 +3776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>261</v>
       </c>
@@ -3782,7 +3784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>273</v>
       </c>
@@ -3790,7 +3792,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>274</v>
       </c>
@@ -3798,7 +3800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>277</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>262</v>
       </c>
@@ -3814,7 +3816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>271</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>263</v>
       </c>
@@ -3830,7 +3832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>279</v>
       </c>
@@ -3838,7 +3840,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>298</v>
       </c>
@@ -3847,6 +3849,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
   <extLst>
@@ -3870,7 +3873,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="122" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" customWidth="1"/>
@@ -3878,12 +3881,13 @@
     <col min="6" max="6" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="56" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>338</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -3907,13 +3911,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.453125" customWidth="1"/>
     <col min="2" max="2" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>205</v>
       </c>
@@ -3921,7 +3925,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3929,7 +3933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3937,7 +3941,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3945,7 +3949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3953,7 +3957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3961,7 +3965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3969,7 +3973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3977,7 +3981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3985,7 +3989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -3993,7 +3997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4001,7 +4005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -4009,7 +4013,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>332</v>
       </c>
@@ -4017,7 +4021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -4025,7 +4029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -4033,7 +4037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -4041,7 +4045,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4049,7 +4053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -4057,7 +4061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4065,7 +4069,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -4073,7 +4077,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -4081,7 +4085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -4089,7 +4093,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -4097,7 +4101,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -4105,7 +4109,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -4113,7 +4117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -4121,7 +4125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -4129,7 +4133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -4137,7 +4141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -4145,7 +4149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -4153,7 +4157,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -4161,7 +4165,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -4169,7 +4173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -4177,7 +4181,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -4185,7 +4189,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -4193,7 +4197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -4201,7 +4205,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -4209,7 +4213,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -4217,7 +4221,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>333</v>
       </c>
@@ -4225,7 +4229,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="28" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>334</v>
       </c>
@@ -4233,7 +4237,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -4241,7 +4245,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -4249,7 +4253,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -4257,7 +4261,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -4273,7 +4277,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -4281,7 +4285,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -4289,7 +4293,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -4297,7 +4301,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -4305,7 +4309,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -4313,7 +4317,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -4321,7 +4325,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -4329,7 +4333,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -4337,7 +4341,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -4345,7 +4349,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -4353,7 +4357,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -4361,7 +4365,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -4369,7 +4373,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -4377,7 +4381,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -4385,7 +4389,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -4393,7 +4397,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -4401,7 +4405,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -4409,7 +4413,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -4417,7 +4421,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -4425,7 +4429,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -4433,7 +4437,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -4441,7 +4445,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -4449,7 +4453,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -4457,7 +4461,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -4473,7 +4477,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -4481,7 +4485,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -4489,7 +4493,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -4497,7 +4501,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -4505,7 +4509,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -4513,7 +4517,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -4521,7 +4525,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -4529,7 +4533,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -4537,7 +4541,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -4545,7 +4549,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -4553,7 +4557,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>160</v>
       </c>
@@ -4561,7 +4565,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -4569,7 +4573,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -4577,7 +4581,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -4585,7 +4589,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>168</v>
       </c>
@@ -4593,7 +4597,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>170</v>
       </c>
@@ -4601,7 +4605,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -4609,7 +4613,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -4617,7 +4621,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -4625,7 +4629,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>178</v>
       </c>
@@ -4633,7 +4637,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -4641,7 +4645,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>182</v>
       </c>
@@ -4649,7 +4653,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -4657,7 +4661,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -4673,7 +4677,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -4681,7 +4685,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>192</v>
       </c>
@@ -4689,7 +4693,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>194</v>
       </c>
@@ -4697,7 +4701,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>198</v>
       </c>
@@ -4713,7 +4717,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>200</v>
       </c>
@@ -4721,7 +4725,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -4729,7 +4733,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -4738,6 +4742,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
@@ -4761,62 +4766,63 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
@@ -4839,29 +4845,30 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.26953125" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -4880,104 +4887,104 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.26953125" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>229</v>
       </c>
@@ -4986,6 +4993,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A19">
     <sortCondition ref="A19"/>
   </sortState>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5005,24 +5013,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5039,14 +5048,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5066,7 +5076,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
@@ -5079,7 +5089,7 @@
     <col min="18" max="18" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>320</v>
       </c>
@@ -5136,6 +5146,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
@@ -5154,7 +5165,7 @@
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7265625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -5176,7 +5187,7 @@
     <col min="22" max="22" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>320</v>
       </c>
@@ -5245,6 +5256,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -5258,7 +5270,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.1796875" customWidth="1"/>
     <col min="2" max="2" width="23.1796875" customWidth="1"/>
@@ -5294,7 +5306,7 @@
     <col min="39" max="39" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>320</v>
       </c>
@@ -5414,6 +5426,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5430,7 +5443,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="25.453125" customWidth="1"/>
@@ -5449,7 +5462,7 @@
     <col min="23" max="23" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>320</v>
       </c>
@@ -5521,6 +5534,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -5542,7 +5556,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="25.453125" customWidth="1"/>
@@ -5559,7 +5573,7 @@
     <col min="20" max="20" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>320</v>
       </c>
@@ -5622,6 +5636,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -5638,7 +5653,7 @@
       <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -5655,7 +5670,7 @@
     <col min="26" max="26" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>320</v>
       </c>
@@ -5736,6 +5751,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5757,7 +5773,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="34.453125" customWidth="1"/>
@@ -5776,7 +5792,7 @@
     <col min="19" max="19" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>320</v>
       </c>
@@ -5836,6 +5852,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5857,7 +5874,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="25.453125" customWidth="1"/>
@@ -5874,7 +5891,7 @@
     <col min="19" max="19" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>320</v>
       </c>
@@ -5934,6 +5951,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>